<commit_message>
updated to use 9th data
</commit_message>
<xml_diff>
--- a/config/emission_factors.xlsx
+++ b/config/emission_factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aperc-my.sharepoint.com/personal/finbar_maunsell_aperc_or_jp/Documents/Documents/Github/aperc-emissions/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APERC\aperc-emissions\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{A9BD8D74-96F9-4EA6-B56F-63CD12E84505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{583D08A3-AD2C-445F-BF99-7B50FA0BE1C5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341D5019-49CA-46EA-94AC-99804105BEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="5205" windowWidth="23010" windowHeight="12330" xr2:uid="{5F4790B2-78FB-46B6-96D5-BBAF6FC748D5}"/>
+    <workbookView xWindow="1755" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{5F4790B2-78FB-46B6-96D5-BBAF6FC748D5}"/>
   </bookViews>
   <sheets>
     <sheet name="IPCC Emission Factors 2021" sheetId="1" r:id="rId1"/>
@@ -429,10 +429,10 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,6 +448,230 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>21166</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>52916</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06818F1E-B67F-D06B-F6C6-F92E63A338AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7387167" y="698500"/>
+          <a:ext cx="5736166" cy="3376083"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>https://chat.openai.com/share/9257d149-c966-4874-9252-241196fc2645</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Note that these values</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> are for carbon content only, not carbon dioxide or carbon dioxide equivalent! The values are timesed by </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>3.67/ to get CO2 emissions factors (One ton of carbon equals 44/12 = 11/3 = 3.67 tons of carbon dioxide).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>This is the line where that happens:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>IPCC_emissions_factors['Emissions factor (MT/PJ)'] = IPCC_emissions_factors*3.67/1000</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -747,21 +971,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BEF2425-9A87-47A9-BB1D-23273F1CF4CD}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="3" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3"/>
-    <col min="5" max="5" width="5.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="35.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" style="3" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" style="3"/>
+    <col min="5" max="5" width="16.7265625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="33" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -772,11 +997,11 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -789,12 +1014,12 @@
       <c r="D2" s="3">
         <v>20.6</v>
       </c>
-      <c r="F2" s="5">
+      <c r="E2" s="5">
         <v>20</v>
       </c>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -807,12 +1032,12 @@
       <c r="D3" s="3">
         <v>23.3</v>
       </c>
-      <c r="F3" s="5">
+      <c r="E3" s="5">
         <v>22</v>
       </c>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -825,12 +1050,12 @@
       <c r="D4" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="F4" s="5">
+      <c r="E4" s="5">
         <v>17.2</v>
       </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -843,12 +1068,12 @@
       <c r="D5" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="F5" s="5">
+      <c r="E5" s="5">
         <v>18.899999999999999</v>
       </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -861,12 +1086,12 @@
       <c r="D6" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="F6" s="5">
+      <c r="E6" s="5">
         <v>19.100000000000001</v>
       </c>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -879,12 +1104,12 @@
       <c r="D7" s="3">
         <v>20.3</v>
       </c>
-      <c r="F7" s="5">
+      <c r="E7" s="5">
         <v>19.100000000000001</v>
       </c>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -897,12 +1122,12 @@
       <c r="D8" s="3">
         <v>20.100000000000001</v>
       </c>
-      <c r="F8" s="5">
+      <c r="E8" s="5">
         <v>19.5</v>
       </c>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -915,12 +1140,12 @@
       <c r="D9" s="3">
         <v>21.6</v>
       </c>
-      <c r="F9" s="5">
+      <c r="E9" s="5">
         <v>19.600000000000001</v>
       </c>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -933,12 +1158,12 @@
       <c r="D10" s="3">
         <v>20.399999999999999</v>
       </c>
-      <c r="F10" s="5">
+      <c r="E10" s="5">
         <v>20</v>
       </c>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -951,12 +1176,12 @@
       <c r="D11" s="3">
         <v>21.5</v>
       </c>
-      <c r="F11" s="5">
+      <c r="E11" s="5">
         <v>20.2</v>
       </c>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -969,12 +1194,12 @@
       <c r="D12" s="3">
         <v>17.899999999999999</v>
       </c>
-      <c r="F12" s="5">
+      <c r="E12" s="5">
         <v>21.1</v>
       </c>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -987,12 +1212,12 @@
       <c r="D13" s="3">
         <v>18.7</v>
       </c>
-      <c r="F13" s="5">
+      <c r="E13" s="5">
         <v>17.2</v>
       </c>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1005,12 +1230,12 @@
       <c r="D14" s="3">
         <v>20.8</v>
       </c>
-      <c r="F14" s="5">
+      <c r="E14" s="5">
         <v>16.8</v>
       </c>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -1023,11 +1248,11 @@
       <c r="D15" s="3">
         <v>24.5</v>
       </c>
-      <c r="F15" s="5">
+      <c r="E15" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1040,11 +1265,11 @@
       <c r="D16" s="3">
         <v>20.5</v>
       </c>
-      <c r="F16" s="5">
+      <c r="E16" s="5">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1057,11 +1282,11 @@
       <c r="D17" s="3">
         <v>31.3</v>
       </c>
-      <c r="F17" s="5">
+      <c r="E17" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1074,11 +1299,11 @@
       <c r="D18" s="3">
         <v>20.9</v>
       </c>
-      <c r="F18" s="5">
+      <c r="E18" s="5">
         <v>27.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -1091,11 +1316,11 @@
       <c r="D19" s="3">
         <v>19</v>
       </c>
-      <c r="F19" s="5">
+      <c r="E19" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1108,11 +1333,11 @@
       <c r="D20" s="3">
         <v>20.3</v>
       </c>
-      <c r="F20" s="5">
+      <c r="E20" s="5">
         <v>15.7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1125,11 +1350,11 @@
       <c r="D21" s="3">
         <v>20.3</v>
       </c>
-      <c r="F21" s="5">
+      <c r="E21" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1142,11 +1367,11 @@
       <c r="D22" s="3">
         <v>20.3</v>
       </c>
-      <c r="F22" s="5">
+      <c r="E22" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1159,11 +1384,11 @@
       <c r="D23" s="3">
         <v>27.5</v>
       </c>
-      <c r="F23" s="5">
+      <c r="E23" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1176,11 +1401,11 @@
       <c r="D24" s="3">
         <v>27.6</v>
       </c>
-      <c r="F24" s="5">
+      <c r="E24" s="5">
         <v>26.8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1193,11 +1418,11 @@
       <c r="D25" s="3">
         <v>27.2</v>
       </c>
-      <c r="F25" s="5">
+      <c r="E25" s="5">
         <v>25.8</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -1210,11 +1435,11 @@
       <c r="D26" s="3">
         <v>27.3</v>
       </c>
-      <c r="F26" s="5">
+      <c r="E26" s="5">
         <v>25.8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -1227,11 +1452,11 @@
       <c r="D27" s="3">
         <v>31.3</v>
       </c>
-      <c r="F27" s="5">
+      <c r="E27" s="5">
         <v>26.2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1244,11 +1469,11 @@
       <c r="D28" s="3">
         <v>34</v>
       </c>
-      <c r="F28" s="5">
+      <c r="E28" s="5">
         <v>27.6</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -1261,11 +1486,11 @@
       <c r="D29" s="3">
         <v>29</v>
       </c>
-      <c r="F29" s="5">
+      <c r="E29" s="5">
         <v>29.1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -1278,11 +1503,11 @@
       <c r="D30" s="3">
         <v>29.6</v>
       </c>
-      <c r="F30" s="5">
+      <c r="E30" s="5">
         <v>25.8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -1295,11 +1520,11 @@
       <c r="D31" s="3">
         <v>29.6</v>
       </c>
-      <c r="F31" s="5">
+      <c r="E31" s="5">
         <v>26.6</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -1312,11 +1537,11 @@
       <c r="D32" s="3">
         <v>32.4</v>
       </c>
-      <c r="F32" s="5">
+      <c r="E32" s="5">
         <v>29.5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -1329,11 +1554,11 @@
       <c r="D33" s="3">
         <v>32.4</v>
       </c>
-      <c r="F33" s="5">
+      <c r="E33" s="5">
         <v>29.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1346,11 +1571,11 @@
       <c r="D34" s="3">
         <v>26</v>
       </c>
-      <c r="F34" s="5">
+      <c r="E34" s="5">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
@@ -1363,11 +1588,11 @@
       <c r="D35" s="3">
         <v>15</v>
       </c>
-      <c r="F35" s="5">
+      <c r="E35" s="5">
         <v>12.1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
@@ -1380,11 +1605,11 @@
       <c r="D36" s="3">
         <v>15</v>
       </c>
-      <c r="F36" s="5">
+      <c r="E36" s="5">
         <v>12.1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
@@ -1397,11 +1622,11 @@
       <c r="D37" s="3">
         <v>84</v>
       </c>
-      <c r="F37" s="5">
+      <c r="E37" s="5">
         <v>70.8</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
@@ -1414,11 +1639,11 @@
       <c r="D38" s="3">
         <v>55</v>
       </c>
-      <c r="F38" s="5">
+      <c r="E38" s="5">
         <v>49.6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
@@ -1431,11 +1656,11 @@
       <c r="D39" s="3">
         <v>15.9</v>
       </c>
-      <c r="F39" s="5">
+      <c r="E39" s="5">
         <v>15.3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A40" s="7" t="s">
         <v>42</v>
       </c>
@@ -1448,11 +1673,11 @@
       <c r="D40" s="3">
         <v>33</v>
       </c>
-      <c r="F40" s="5">
+      <c r="E40" s="5">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
@@ -1465,11 +1690,11 @@
       <c r="D41" s="3">
         <v>50</v>
       </c>
-      <c r="F41" s="5">
+      <c r="E41" s="5">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
@@ -1482,11 +1707,11 @@
       <c r="D42" s="3">
         <v>20.3</v>
       </c>
-      <c r="F42" s="5">
+      <c r="E42" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
@@ -1499,11 +1724,11 @@
       <c r="D43" s="3">
         <v>29.5</v>
       </c>
-      <c r="F43" s="5">
+      <c r="E43" s="5">
         <v>28.9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
@@ -1516,11 +1741,11 @@
       <c r="D44" s="3">
         <v>36</v>
       </c>
-      <c r="F44" s="5">
+      <c r="E44" s="5">
         <v>30.5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>47</v>
       </c>
@@ -1533,11 +1758,11 @@
       <c r="D45" s="3">
         <v>30</v>
       </c>
-      <c r="F45" s="5">
+      <c r="E45" s="5">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>48</v>
       </c>
@@ -1550,11 +1775,11 @@
       <c r="D46" s="3">
         <v>32</v>
       </c>
-      <c r="F46" s="5">
+      <c r="E46" s="5">
         <v>29.9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
@@ -1567,11 +1792,11 @@
       <c r="D47" s="3">
         <v>36</v>
       </c>
-      <c r="F47" s="5">
+      <c r="E47" s="5">
         <v>30.5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>50</v>
       </c>
@@ -1584,11 +1809,11 @@
       <c r="D48" s="3">
         <v>23</v>
       </c>
-      <c r="F48" s="5">
+      <c r="E48" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>51</v>
       </c>
@@ -1601,11 +1826,11 @@
       <c r="D49" s="3">
         <v>23</v>
       </c>
-      <c r="F49" s="5">
+      <c r="E49" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>52</v>
       </c>
@@ -1618,11 +1843,11 @@
       <c r="D50" s="3">
         <v>26</v>
       </c>
-      <c r="F50" s="5">
+      <c r="E50" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>53</v>
       </c>
@@ -1635,11 +1860,11 @@
       <c r="D51" s="3">
         <v>18</v>
       </c>
-      <c r="F51" s="5">
+      <c r="E51" s="5">
         <v>14.9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>54</v>
       </c>
@@ -1652,11 +1877,11 @@
       <c r="D52" s="3">
         <v>18</v>
       </c>
-      <c r="F52" s="5">
+      <c r="E52" s="5">
         <v>14.9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>55</v>
       </c>
@@ -1669,11 +1894,11 @@
       <c r="D53" s="3">
         <v>18</v>
       </c>
-      <c r="F53" s="5">
+      <c r="E53" s="5">
         <v>30.6</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>56</v>
       </c>
@@ -1686,11 +1911,11 @@
       <c r="D54" s="3">
         <v>32</v>
       </c>
-      <c r="F54" s="5">
+      <c r="E54" s="5">
         <v>27.3</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
@@ -1703,16 +1928,16 @@
       <c r="D55" s="3">
         <v>0</v>
       </c>
-      <c r="F55" s="1">
+      <c r="E55" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="8" t="s">
         <v>59</v>
       </c>
@@ -1720,6 +1945,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1734,26 +1960,26 @@
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1767,7 +1993,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1791,28 +2017,28 @@
   <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="3" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3"/>
-    <col min="5" max="5" width="5.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="35.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" style="3" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" style="3"/>
+    <col min="5" max="5" width="5.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" ht="33" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1827,7 +2053,7 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1842,7 +2068,7 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1857,7 +2083,7 @@
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1872,7 +2098,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1887,7 +2113,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1902,7 +2128,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1917,7 +2143,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1932,7 +2158,7 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1947,7 +2173,7 @@
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1962,7 +2188,7 @@
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1977,7 +2203,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1992,7 +2218,7 @@
       </c>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2007,7 +2233,7 @@
       </c>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -2022,7 +2248,7 @@
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -2037,7 +2263,7 @@
       </c>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2052,7 +2278,7 @@
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2067,7 +2293,7 @@
       </c>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2082,7 +2308,7 @@
       </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -2097,7 +2323,7 @@
       </c>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -2112,7 +2338,7 @@
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -2127,7 +2353,7 @@
       </c>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -2142,7 +2368,7 @@
       </c>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -2157,7 +2383,7 @@
       </c>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -2172,7 +2398,7 @@
       </c>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -2187,7 +2413,7 @@
       </c>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -2202,7 +2428,7 @@
       </c>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -2217,7 +2443,7 @@
       </c>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -2232,7 +2458,7 @@
       </c>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -2247,7 +2473,7 @@
       </c>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -2262,7 +2488,7 @@
       </c>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -2277,7 +2503,7 @@
       </c>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -2292,7 +2518,7 @@
       </c>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -2307,7 +2533,7 @@
       </c>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -2322,7 +2548,7 @@
       </c>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
@@ -2337,7 +2563,7 @@
       </c>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
@@ -2352,7 +2578,7 @@
       </c>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
@@ -2367,7 +2593,7 @@
       </c>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
@@ -2382,7 +2608,7 @@
       </c>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -2397,7 +2623,7 @@
       </c>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="33" x14ac:dyDescent="0.45">
       <c r="A41" s="7" t="s">
         <v>42</v>
       </c>
@@ -2411,7 +2637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
@@ -2425,7 +2651,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
@@ -2439,7 +2665,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
@@ -2453,7 +2679,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -2467,7 +2693,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
@@ -2481,7 +2707,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -2496,7 +2722,7 @@
       </c>
       <c r="F47" s="10"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -2510,7 +2736,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -2525,7 +2751,7 @@
       </c>
       <c r="F49" s="9"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -2540,7 +2766,7 @@
       </c>
       <c r="F50" s="9"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -2555,7 +2781,7 @@
       </c>
       <c r="F51" s="9"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -2569,7 +2795,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
@@ -2583,7 +2809,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
@@ -2598,7 +2824,7 @@
       </c>
       <c r="F54" s="9"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
@@ -2612,7 +2838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -2626,10 +2852,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="8"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="8"/>
     </row>
   </sheetData>

</xml_diff>